<commit_message>
adding teachers to excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/public/FirstYear.xlsx
+++ b/src/main/resources/public/FirstYear.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2352" uniqueCount="79">
   <si>
     <t>CSE</t>
   </si>
@@ -148,6 +148,114 @@
   </si>
   <si>
     <t xml:space="preserve">M201(T)  /  </t>
+  </si>
+  <si>
+    <t>HU291[SDa]  /  MOOCS[]</t>
+  </si>
+  <si>
+    <t>M201[ABj]  /  []</t>
+  </si>
+  <si>
+    <t>CH201[SC, PD]  /  []</t>
+  </si>
+  <si>
+    <t>CS201[GY]  /  []</t>
+  </si>
+  <si>
+    <t>ME291[TR, TKG]  /  []</t>
+  </si>
+  <si>
+    <t>HU201[SDa]  /  []</t>
+  </si>
+  <si>
+    <t>CS291[GY, AH]  /  M201(T)[ABj]</t>
+  </si>
+  <si>
+    <t>IT291[RG, ARC]  /  M201(T)[SCh]</t>
+  </si>
+  <si>
+    <t>IT201[AKS]  /  []</t>
+  </si>
+  <si>
+    <t>CH201[PD]  /  []</t>
+  </si>
+  <si>
+    <t>PH201[SoM]  /  []</t>
+  </si>
+  <si>
+    <t>ECE291[SDe, SSK]  /  M201(T)[SCh]</t>
+  </si>
+  <si>
+    <t>ECE201[SMa]  /  []</t>
+  </si>
+  <si>
+    <t>M201[SCh]  /  []</t>
+  </si>
+  <si>
+    <t>PH201(T)[AT, SoM]  /  []</t>
+  </si>
+  <si>
+    <t>ME291[BDC]  /  []</t>
+  </si>
+  <si>
+    <t>EE291[AKS, SL]  /  PH201(T)[AT, SoM]</t>
+  </si>
+  <si>
+    <t>EE201[SL]  /  []</t>
+  </si>
+  <si>
+    <t>M201(T)[SCh]  /  []</t>
+  </si>
+  <si>
+    <t>PH201[AT]  /  []</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS201[GY]  /  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M201[ABj]  /  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH201[SC, PD]  /  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME291[TR, TKG]  /  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HU201[SDa]  /  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH201[PD]  /  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT201[AKS]  /  </t>
+  </si>
+  <si>
+    <t>IT291[AKS, ARC]  /  M201(T)[SCh]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECE201[SMa]  /  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M201[SCh]  /  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH201[SoM]  /  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH201(T)[AT, SoM]  /  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME291[BDC]  /  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH201[AT]  /  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M201(T)[SCh]  /  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE201[SL]  /  </t>
   </si>
 </sst>
 </file>
@@ -489,25 +597,25 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5">
@@ -517,25 +625,25 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7">
@@ -545,25 +653,25 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9">
@@ -573,22 +681,22 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="G10" t="s">
         <v>12</v>
@@ -601,25 +709,25 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
@@ -639,25 +747,25 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="G16" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
@@ -667,25 +775,25 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="F18" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="G18" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19">
@@ -695,22 +803,22 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="G20" t="s">
         <v>12</v>
@@ -723,25 +831,25 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="E22" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="F22" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="G22" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23">
@@ -751,25 +859,25 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="F24" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="G24" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25">
@@ -789,25 +897,25 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="E28" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="F28" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="G28" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29">
@@ -817,25 +925,25 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="D30" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="E30" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F30" t="s">
         <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31">
@@ -845,25 +953,25 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="E32" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="G32" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33">
@@ -873,25 +981,25 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="E34" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="F34" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35">
@@ -901,25 +1009,25 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="D36" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="E36" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="F36" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="G36" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37">
@@ -939,25 +1047,25 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="E40" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="F40" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="G40" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41">
@@ -967,25 +1075,25 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="D42" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="E42" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="F42" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="G42" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43">
@@ -998,22 +1106,22 @@
         <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="C44" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="D44" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="E44" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="F44" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="G44" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45">
@@ -1023,25 +1131,25 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="E46" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="F46" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="G46" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47">
@@ -1051,25 +1159,25 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="D48" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="E48" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="F48" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="G48" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>